<commit_message>
change in exel files
</commit_message>
<xml_diff>
--- a/downloads/excel-templates/questions_blanks_template.xlsx
+++ b/downloads/excel-templates/questions_blanks_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\exam\public\downloads\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\awd\xampp\htdocs\schoolsysrepo\downloads\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,16 +17,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$N$2:$N$3</definedName>
-    <definedName name="question_type">Sheet1!$N$2:$N$3</definedName>
-    <definedName name="type">Sheet1!$N$2:$N$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$O$2:$O$3</definedName>
+    <definedName name="question_type">Sheet1!$O$2:$O$3</definedName>
+    <definedName name="type">Sheet1!$O$2:$O$6</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>subject_id</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Telangana,Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>academic_id</t>
+  </si>
+  <si>
+    <t>course_id</t>
+  </si>
+  <si>
+    <t>sem_id</t>
   </si>
 </sst>
 </file>
@@ -412,81 +421,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>17</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>